<commit_message>
completato relazioni libro + sanificated con libroexportDto
</commit_message>
<xml_diff>
--- a/file-storage/ExportDataLibro.xlsx
+++ b/file-storage/ExportDataLibro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>libroId</t>
   </si>
@@ -38,16 +38,43 @@
     <t>copie</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Il Signore degli Anelli</t>
+  </si>
+  <si>
+    <t>J.R.R. Tolkien</t>
+  </si>
+  <si>
+    <t>1234561954123</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Un'edizione</t>
+  </si>
+  <si>
+    <t>1954</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Il mistero del tesoro scomparso</t>
   </si>
   <si>
     <t>Geronimo Stilton</t>
   </si>
   <si>
-    <t>978-88-565-0061-0</t>
+    <t>978-88-565-2015-0</t>
   </si>
   <si>
     <t>Avventura</t>
@@ -62,64 +89,31 @@
     <t>10</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Il Grande Gatsby</t>
-  </si>
-  <si>
-    <t>F. Scott Fitzgerald</t>
-  </si>
-  <si>
-    <t>978-3-16-148410-0</t>
-  </si>
-  <si>
-    <t>Romanzo</t>
-  </si>
-  <si>
-    <t>Scribner</t>
-  </si>
-  <si>
-    <t>1925</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Geronimo Stilton: Viaggio nel Tempo</t>
-  </si>
-  <si>
-    <t>9780545011724</t>
-  </si>
-  <si>
-    <t>Edizioni Piemme</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Il Signore degli Anelli</t>
-  </si>
-  <si>
-    <t>J.R.R. Tolkien</t>
-  </si>
-  <si>
-    <t>1234561954123</t>
-  </si>
-  <si>
-    <t>Fantasy</t>
-  </si>
-  <si>
-    <t>Un'edizione</t>
-  </si>
-  <si>
-    <t>1954</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Il codice Da Vinci</t>
+  </si>
+  <si>
+    <t>Dan Brown</t>
+  </si>
+  <si>
+    <t>978-88-459-2003-5</t>
+  </si>
+  <si>
+    <t>Thriller</t>
+  </si>
+  <si>
+    <t>Mondadori</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -224,106 +218,106 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>16</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>24</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="F5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="G5" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="H5" t="s" s="0">
         <v>32</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="G6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="H6" t="s" s="0">
         <v>32</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>